<commit_message>
:bug: fix: all test run fine now
</commit_message>
<xml_diff>
--- a/tests/mismatches_detailed.xlsx
+++ b/tests/mismatches_detailed.xlsx
@@ -429,7 +429,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Label</t>
+          <t>Label_sample</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -439,7 +439,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>label</t>
+          <t>Label_processed</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">

</xml_diff>

<commit_message>
:bug: fix: Correct baseline NER evaluation and simplify module imports in examples by adjusting sys.path.
</commit_message>
<xml_diff>
--- a/tests/mismatches_detailed.xlsx
+++ b/tests/mismatches_detailed.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,14 +480,15 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Prezados bom dia,  Em visita ao Hospital de Apoio de Brasilia onde fui recepcionada e bem atendida pelo Dr Joaquim fui orientada sobre a existência de dados abertos e painel de atenção ao CiD G-10. Neste sentido solicito informação quanto ao perfil do cidadão acometido pela doença de Huntington no Distrito Federal.  Taxa de pacientes atendidos por idade extraidas do Infosaúde do DF.   Solicito o caminho de acesso ao dado aberto público.  Atenciosamente,  Antonio Costa Controladoria-Geral do Distrito Federal Gestor PPGG 21-1205-1999</t>
+          <t>Prezados senhores, boa tarde!
+Solicito acesso integral aos autos do Processo SEI 00015-01009853/2026-01, com urgência, visto a decorrência de prazo em andamento.</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -497,19 +498,19 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -519,24 +520,24 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Sou inquilina do imóvel localizado na CRN 104 Bloco I loja 15, em frente à L3 sul, onde o GDF tem feito o trabalho asfalto.  No referido imóvel há inúmeros vitrais (imagens anexas), painéis Athos Bulsão, mosaicos de Gugon e lustres e luminárias antigas, os quais têm passado por intensa movimentação em razão do maquinário usado pelo GDF na obra; o que coloca as peças em risco.  Assim, visando a prevenir responsabilidades, venho por intermédio deste canal noticiar os fatos, ao tempo em que pugno pela adoção de cautelas devidas na execução do serviço a fim de evitar danos irreparáveis às referidas obras.</t>
+          <t>Cidadã, solicita acesso aos autos do processo SEI 00015-00568900/2016-56, haja vista que tal processo versa sobre uma denúncia que fez, no entanto, não lhe fora disponibilizado nenhum documento resultante da apuração.</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -545,31 +546,31 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>False Negative</t>
+          <t>False Positive</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Bom dia!! Gostariabde uma fiscalização nas calçadas na shdf 602 - 607, blocos R U J C F. Grata</t>
+          <t>Prezados bom dia,  Em visita ao Hospital de Apoio de Brasilia onde fui recepcionada e bem atendida pelo Dr Joaquim fui orientada sobre a existência de dados abertos e painel de atenção ao CiD G-10. Neste sentido solicito informação quanto ao perfil do cidadão acometido pela doença de Huntington no Distrito Federal.  Taxa de pacientes atendidos por idade extraidas do Infosaúde do DF.   Solicito o caminho de acesso ao dado aberto público.  Atenciosamente,  Antonio Costa Controladoria-Geral do Distrito Federal Gestor PPGG 21-1205-1999</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -581,28 +582,106 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>False Negative</t>
+          <t>False Positive</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
+        <v>15</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Sou inquilina do imóvel localizado na CRN 104 Bloco I loja 15, em frente à L3 sul, onde o GDF tem feito o trabalho asfalto.  No referido imóvel há inúmeros vitrais (imagens anexas), painéis Athos Bulsão, mosaicos de Gugon e lustres e luminárias antigas, os quais têm passado por intensa movimentação em razão do maquinário usado pelo GDF na obra; o que coloca as peças em risco.  Assim, visando a prevenir responsabilidades, venho por intermédio deste canal noticiar os fatos, ao tempo em que pugno pela adoção de cautelas devidas na execução do serviço a fim de evitar danos irreparáveis às referidas obras.</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>False Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>18</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Bom dia!! Gostariabde uma fiscalização nas calçadas na shdf 602 - 607, blocos R U J C F. Grata</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>False Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
         <v>22</v>
       </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="inlineStr">
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
         <is>
           <t>Prezados,
 1) Solicitamos informações deste órgão ou entidade sobre o real quantitativo de servidores de carreira (efetivos)
@@ -628,121 +707,43 @@
 Agradecemos o envio das informações.</t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="inlineStr">
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="inlineStr">
         <is>
           <t>False Negative</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>25</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Por qual motivo o Processo Sei nº 00589-01245698/2025-15 não foi atendido até o presente MOMENTO? ELE ESTA PARADO DESDE O DIA 10/05/2025 CONFORME ANEXO.</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>False Negative</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>47</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Ref.:  Processo SEI nº  0025-000598/2006    Ilustres Servidores do Departamento de Trânsito do DF,  Cumprimentando-os cordialmente, o escritório Cassandra Rodrigues Advogados Associados, vem, por meio deste advogado que este subscreve, representando os interesses da WT VIDA EMPREENDIMENTOS IMOBILIÁRIOS LTDA., expor e requerer o quanto segue.  Nos termos do artigo 7º, inciso XV do Estatuto da Ordem dos Advogados do Brasil (Lei nº 8.906/94) é direito do advogado ter vista dos processos judiciais ou administrativos de qualquer natureza, em cartório ou na repartição competente, ou retirá-los pelos prazos legais.  Cumpre invocar também o disposto no artigo 5º, inciso XXXIII, artigo 37, §3º, inciso II e artigo 216, §2º da Constituição Federal, bem como na Lei 12.527/2011, que garantem o acesso à informação.   Desta feita, considerando que nos autos do processo em epígrafe constam documentos que não foram fornecidos quando solicitados e, tendo em vista a previsão legal supracitada, requer-se o acesso à seguinte documentação, em caráter de urgência:  2.png  Ademais, encaminho o instrumento de procuração, em anexo, por meio do qual a WT VIDA EMPREENDIMENTOS IMOBILIÁRIOS LTDA. outorga poderes para este escritório representá-lo perante órgãos e repartições públicas do Governo do Distrito Federal.  Desde já agradecemos pela atenção e disponibilidade e aguardamos retorno por parte de vossas senhorias.  Atenciosamente,</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>False Positive</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Inteligência Artificial e Letramento Digital no Setor Público  Prezado(a) servidor(a),  Este questionário tem como objetivo mapear as percepções sobre habilidades relacionadas ao letramento digital e ao uso de Inteligência Artificial Generativa no setor público. Dividido em três seções – Perfil Demográfico e Profissional, Letramento Digital e Inteligência Artificial Generativa – o estudo oferece insights valiosos para que governos identifiquem desafios e oportunidades na busca por inovação e transformação digital. Os benefícios são significativos, pois os participantes podem identificar suas necessidades de capacitação, enquanto os governos utilizam os resultados para mapear lacunas e desenvolver estratégias mais eficazes para promover a inclusão digital, superando os obstáculos associados à adoção de novas tecnologias. Solicita-se, portanto, ampla divulgação nos órgãos do Governo do Distrito Federal, a fim de garantir resultados robustos e relevantes.  O tempo estimado para responder é de 5 a 10 minutos. Todas as respostas são confidenciais, pois nenhum dado que identifique o participante será coletado, garantindo sua privacidade e anonimato. As informações serão utilizadas exclusivamente para fins de pesquisa no âmbito do Mestrado da Escola de Políticas Públicas e Governo do Instituto Brasileiro de Ensino, Desenvolvimento e Pesquisa .  Acesse o questionário pelo link: https://bit.ly/4gkOtWa  A sua opinião importa! Contamos com a sua participação.   Desde já, agradecemos a sua colaboração.  Cordialmente,  Carolina Guimarães Neves: Atividade de Defesa do Consumidor e Fiscal de Defesa do Consumidor. Pesquisadora do Instituto Brasileiro de Ensino, Desenvolvimento e Pesquisa. Orientador: Profª. Doutorª. Fátima Lima</t>
+          <t>Solicito informação a respeito da existência bens tombados a nível distrital que possam gerar área envoltória e/ou restrições urbanísticas para novas construções que possam atingir o imóvel de interesse localizado no seguinte endereço: Comercial II, Rua 41, Lo 20, CEP 20031 - 900, com inscrição imobiliária nº 78965412  e matrícula nº 654.789 8ºRI. A informação é para fins de Estudo de Viabilidade Técnica e Legal - EVTL para empreendimento comercial.</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -761,10 +762,10 @@
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
@@ -774,12 +775,367 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
+        <v>31</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>informações sobre o processo : 12398-00000018/2015-23 adasa df</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>False Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>32</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Boa Tarde,
+Gostaria de informação sobre processo iniciado na Polícia Civil do DF e não teve resposta concreta até o momento
+Processo n° 10259-65478321/2018-25
+Processo n° 10259-65478441/2018-56
+Grato.</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>False Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>33</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>SOLICITO ACESSO AO PROCESSO SEI 00258-36985274/2017-43</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>False Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>38</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Boa tarde! Gostaria de consultar o andamento do processo nº 589642/2018-58 realizado em 02/09/2018, solicitando a isenção da TFE ref. o ano 2018 da empresa CARLA PATRICIA GONÇALVES LTDA CNPJ: 25.598.301/0001-68. Solicitação realizada presencialmente na unidade da Terracap na Adm. do Jardim Botânico/DF.   Desde já agradeço.</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>False Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>39</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Solicito cópia do processo 05896-00000589/2017-93 e 00089-98563214/2017-01, que versam sobre a reestruturação da carreira da Assistência Judiciária.</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>False Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>40</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Venho solicitar acesso externo ao processo nº 00256-25631478/2022-34 referente ao Termo de Acordo de Cooperação 25/2022 - AC 25/2022 firmado entre a Secretaria de Estado de Obras e Infraestrutura – SO/DF e a Sistema de Cooperativas Financeiras do Brasil - SICOOB. Segue anexo procuração em meu nome para representar a SICOOB junto à SO/DF, e Termo de Acordo de Concordância. Segue também cópia da CNH digital e comprovante de endereço</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>False Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>47</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Ref.:  Processo SEI nº  0025-000598/2006    Ilustres Servidores do Departamento de Trânsito do DF,  Cumprimentando-os cordialmente, o escritório Cassandra Rodrigues Advogados Associados, vem, por meio deste advogado que este subscreve, representando os interesses da WT VIDA EMPREENDIMENTOS IMOBILIÁRIOS LTDA., expor e requerer o quanto segue.  Nos termos do artigo 7º, inciso XV do Estatuto da Ordem dos Advogados do Brasil (Lei nº 8.906/94) é direito do advogado ter vista dos processos judiciais ou administrativos de qualquer natureza, em cartório ou na repartição competente, ou retirá-los pelos prazos legais.  Cumpre invocar também o disposto no artigo 5º, inciso XXXIII, artigo 37, §3º, inciso II e artigo 216, §2º da Constituição Federal, bem como na Lei 12.527/2011, que garantem o acesso à informação.   Desta feita, considerando que nos autos do processo em epígrafe constam documentos que não foram fornecidos quando solicitados e, tendo em vista a previsão legal supracitada, requer-se o acesso à seguinte documentação, em caráter de urgência:  2.png  Ademais, encaminho o instrumento de procuração, em anexo, por meio do qual a WT VIDA EMPREENDIMENTOS IMOBILIÁRIOS LTDA. outorga poderes para este escritório representá-lo perante órgãos e repartições públicas do Governo do Distrito Federal.  Desde já agradecemos pela atenção e disponibilidade e aguardamos retorno por parte de vossas senhorias.  Atenciosamente,</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>False Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>52</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Inteligência Artificial e Letramento Digital no Setor Público  Prezado(a) servidor(a),  Este questionário tem como objetivo mapear as percepções sobre habilidades relacionadas ao letramento digital e ao uso de Inteligência Artificial Generativa no setor público. Dividido em três seções – Perfil Demográfico e Profissional, Letramento Digital e Inteligência Artificial Generativa – o estudo oferece insights valiosos para que governos identifiquem desafios e oportunidades na busca por inovação e transformação digital. Os benefícios são significativos, pois os participantes podem identificar suas necessidades de capacitação, enquanto os governos utilizam os resultados para mapear lacunas e desenvolver estratégias mais eficazes para promover a inclusão digital, superando os obstáculos associados à adoção de novas tecnologias. Solicita-se, portanto, ampla divulgação nos órgãos do Governo do Distrito Federal, a fim de garantir resultados robustos e relevantes.  O tempo estimado para responder é de 5 a 10 minutos. Todas as respostas são confidenciais, pois nenhum dado que identifique o participante será coletado, garantindo sua privacidade e anonimato. As informações serão utilizadas exclusivamente para fins de pesquisa no âmbito do Mestrado da Escola de Políticas Públicas e Governo do Instituto Brasileiro de Ensino, Desenvolvimento e Pesquisa .  Acesse o questionário pelo link: https://bit.ly/4gkOtWa  A sua opinião importa! Contamos com a sua participação.   Desde já, agradecemos a sua colaboração.  Cordialmente,  Carolina Guimarães Neves: Atividade de Defesa do Consumidor e Fiscal de Defesa do Consumidor. Pesquisadora do Instituto Brasileiro de Ensino, Desenvolvimento e Pesquisa. Orientador: Profª. Doutorª. Fátima Lima</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>False Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>55</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Solicito acesso ao processo 01235-36965412/2025-02</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>False Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
         <v>56</v>
       </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="inlineStr">
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="inlineStr">
         <is>
           <t>Casei recentemente e embora não mudei meu nome civil, necessito retirar novos documentos para mudar o estado civil neles:
 RG, CPF, CNH, Carteira de trabalho, Título de Eleitor e Reservista.
@@ -787,225 +1143,592 @@
 Gostaria de saber os custos e como posso regularizar minha situação.</t>
         </is>
       </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" t="inlineStr">
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="inlineStr">
         <is>
           <t>False Negative</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="n">
+    <row r="19">
+      <c r="A19" t="n">
+        <v>57</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Prezado(a),  Solicito gentilmente à RA XXX - Sul disponibilizar a planta do meu imóvel localizado na Arts 60 – 4 e 14, Aeroporto Niterói, CEP 35800 - 900, com inscrição IPTU nº 456321852 .  Segue matrícula do imóvel.  Grata!  No aguardo.</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>False Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
         <v>62</v>
       </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="inlineStr">
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="inlineStr">
         <is>
           <t>Bom dia,   Eu ja tenho a viabilidade aprovada. porém a junta me pede para eu fazer uma nova viabilidade alegando o nome da empresa!  neste caso o número protocolo integrado vai mudar e a taxa foi paga como faço para aproveitamento a viabilidade aprovada e só atualizar o nome e as exigência da junta comercial. Pois pelo que eu entendo para eu fazer uma nova viabilidade tenho que cancelar a que está vigente, fazer uma nova com certeza terá outro número e como vou fazer com a taxa paga.  motivo pendência nota explicativa 1. corrigir nire: 7893214568-7 89- prezado senhor usuário, orientamos fazer uma nova viabilidade de nome empresarial e retirar o ( 01 ) constante após a natureza jurídica do nome empresarial  CO S DE E Ltda  Preciso de orientação em referencia a taxa que foi pago com o protocolo DFP4568523652, COMO MANTER ENTE NUMERO</t>
         </is>
       </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" t="inlineStr">
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="inlineStr">
         <is>
           <t>False Negative</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="n">
+    <row r="21">
+      <c r="A21" t="n">
         <v>65</v>
       </c>
-      <c r="B11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" t="inlineStr">
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="inlineStr">
         <is>
           <t>Por gentileza,   Gostaria de obter dados de violência psicológica contra a mulher de 2015 a 2025. Estou fazendo uma pesquisa de mestrado e gostaria de fazer essa comparação antes da pandemia.    Grata Conceição Sampaio</t>
         </is>
       </c>
-      <c r="D11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>1</v>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>False Positive</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>False Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>66</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Solicito o envio da Certidão (negativa, positiva, explicativa) da Future Automação e Dados Ltda, CNPJ 56.478.854/0001-24, processo nº 00256-12558945/2019-32.</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>1</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>False Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>67</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Bom dia.
+Preciso ter acesso a um processo meu, no Der, para ver o prazo para recurso. Quais os passos?
+Número do processo: 47856-00236987/2026-54</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>1</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>False Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>71</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Prezados(as),
+Por gentileza, solicito acesso ao processo número SEI: 00254-78541261/2018-95
+O processo envolve o meu nome!
+Obrigada.</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>1</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>False Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>72</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Solicito acesso à integra de processo de meu interesse número  00254-00000684/2024-36, atualmente no DER/DG/CONV/GEN/NUE</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>1</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>False Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
         <v>76</v>
       </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" t="inlineStr">
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="inlineStr">
         <is>
           <t>ILUSTRÍSSIMO SENHOR SECRETÁRIO DA SECRETARIA DE ESTADO DE DESENVOLVIMENTO URBANO E HABITAÇÃO - SEDUH  Ref.: PROCESSO SEI nº 00237-14235698/2021-31  José Paulo Lacerda Almeida, já devidamente qualificado nos autos do processo em epígrafe, vem, respeitosamente e com o acatamento de estilo, à presença de Vossa Excelência, por intermédio de seu advogado, Paulo SA AN Martins, inscrito na OAB/RJ 15.753, com fundamento nos artigos 5º, XXXIII, 37, §3º, II e 216, todos da Constituição Federal, no artigo 3º, I da Lei de Acesso à Informação (Lei nº 12.527/11) bem como, nos artigos 2º, V, VII, e X, e 68 da Lei 9.704/99, requerer a renovação de acesso aos autos do processo em epígrafe, para que o requerente possa apresentar defesas, recursos e se manifestar na integra do processo.</t>
         </is>
       </c>
-      <c r="D12" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>1</v>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>False Positive</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>1</v>
+      </c>
+      <c r="J26" t="n">
+        <v>1</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>False Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
         <v>78</v>
       </c>
-      <c r="B13" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" t="inlineStr">
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="inlineStr">
         <is>
           <t>Sou Residente de Saúde Coletiva da UFRJ e estou fazendo um trabalho sobre dispensação e financiamento de medicamentos hormônais para pessoas trans. Questiono sobre se algum equipamento da prefeitura de Candangolândia e Brasília fornece e dispensa hormônios para hormonização de pessoas trans e qual é a forma de financiamento?</t>
         </is>
       </c>
-      <c r="D13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
-        <v>1</v>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>False Positive</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
+      <c r="D27" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>False Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
         <v>82</v>
       </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" t="inlineStr">
+      <c r="B28" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" t="inlineStr">
         <is>
           <t>Moro na Área Delta, Lt 105 e quero saber quem é o prefeito da quadra e forma de contatá-lo em seu cargo. E também quero receber digitalmente toda a legislação existente definindo e regulamentando a escolha e as atribuições do prefeito da quadra no plano piloto do Distrito Federal</t>
         </is>
       </c>
-      <c r="D14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" t="inlineStr">
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="inlineStr">
         <is>
           <t>False Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>86</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Eu solicito acesso externo cópia integral do processo SEI 0035-15329875/2017-75.
+MOTIVO:
+Em decorrência do Auto De Infração Demolitória nº H-1564-685324-OEU.
+Em caráter de urgência, considerando tenho prazo de 25 dias a partir de 27.02.2022 para interpor recurso.</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" t="n">
+        <v>1</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>False Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>88</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Solicito o acesso aos autos do Processo Administrativo Nº 00025-45625713/2019-85 protocolado no SEE/SUAG/CLOG/DIAP/NPR. Em que o teor é o requerimento de uma agenda com o Governador para receber as associações representativas de interessados direta e indiretamente no projeto de concessão da Rodoviária do Plano Piloto.</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>False Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>93</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Segundo o item 15.4.1 do Edital Concurso Público Nº 02/2026 - ACI, o candidato matriculado no curso de formação profissional percebe, a título de ajuda financeira, 50% (cinquenta por cento) do vencimento básico fixado para o padrão inicial do cargo, até a data de desligamento do curso de formação profissional, com base nesse item, solicito esclarecimentos da CGDF-DF se existe alguma ilegalidade ou impedimento para recebimento da ajuda financeira por candidatos que sejam servidores efetivos de outros entes federativos (União, Estados ou Municípios), que estejam em gozo de férias ou licença não remunerada para participar do curso de formação profissional do referido certame. Além disso, havendo impedimento legal, solicito orientação da CGDF-DF sobre como proceder durante a matrícula no curso de formação, para dirimir as dúvidas dos candidatos que se encontram nessa situação.
+Numa solicitação anterior à SEEC - Protocolo LAI-258453/2026 (328647128), foi informado que:
+Assunto: Protocolo LAI-258453/2026
+1. Trata-se do Despacho ? SEEC/GAB/OUV (687532419), referente ao Protocolo LAI-258453/2026 (328647128), por meio do qual o interessadonsolicita informações sobre matrícula no curso de formação para o servidor efetivo de outros entes federativos (União, Estados ou Municípios),
+especialmente acerca da ajuda financeira, disposto no Edital Concurso Público Nº 02/2026 - ACI.
+2. Assim, entende-se, que a consulta em tela deve ser encaminhada à unidade de gestão de pessoas do órgão de lotação do requerente, para que, à luz da legislação vigente, seja avaliada a possibilidade ou não do recebimento do valor da ajuda financeira referente ao curso de formação.
+3. Em face das considerações apresentadas, encaminho os autos a essa Unidade para conhecimento e providências pertinentes.
+Diante dessa resposta emitida pela SEEC, encaminho para a CGDF-DF novo pedido de informações a respeito do questionamento em tela, visto que o cargo para o qual concorro no certame (Auditor de Controle Interno)  faz parte da estrutura desta secretaria.
+Atenciosamente,</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>1</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>False Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>98</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Não consigo ter acesso ao Processo SEI 02510-25698413/2017-65 no Der que trata de reclamação sobre multa e apreensão indevida de carro. Não tenho acesso à conclusão do processo e decisão final do der.</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>1</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>False Positive</t>
         </is>
       </c>
     </row>

</xml_diff>